<commit_message>
[02/29] ModelItem.Data 가공 및 EquipmentData.cs 추가
</commit_message>
<xml_diff>
--- a/Assets/08.Tables/Excel/Weapon.xlsx
+++ b/Assets/08.Tables/Excel/Weapon.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -38,6 +38,9 @@
     <t xml:space="preserve">equip_holder</t>
   </si>
   <si>
+    <t xml:space="preserve">able_equip_shield</t>
+  </si>
+  <si>
     <t xml:space="preserve">long</t>
   </si>
   <si>
@@ -53,16 +56,25 @@
     <t xml:space="preserve">string</t>
   </si>
   <si>
+    <t xml:space="preserve">bool</t>
+  </si>
+  <si>
     <t xml:space="preserve">OneHand</t>
   </si>
   <si>
     <t xml:space="preserve">OneHandSheathHolder</t>
   </si>
   <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
     <t xml:space="preserve">TwoHand</t>
   </si>
   <si>
     <t xml:space="preserve">TwoHandSheathHolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">XXX / YY / ZZZZ</t>
@@ -380,7 +392,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,32 +420,36 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>20101001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>10</v>
@@ -442,16 +458,18 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>20101002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>12</v>
@@ -460,16 +478,18 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>20102001</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>15</v>
@@ -478,9 +498,11 @@
         <v>0.8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -521,31 +543,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>